<commit_message>
a pruebas agregado el abrir csv y copiar datos al xlsx
</commit_message>
<xml_diff>
--- a/Tests/Config.xlsx
+++ b/Tests/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vya00\Documents\RenewSolutions\Proceso descarga de reportes diarios\Consumidor - Proceso de Descarga de Reportes Diarios Customer Service\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -89,15 +89,15 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="16"/>
+    <phoneticPr fontId="17"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="16"/>
+    <phoneticPr fontId="17"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="16"/>
+    <phoneticPr fontId="17"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -378,9 +378,6 @@
     <t>C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Data\Temp\Despachos to date.xlsx</t>
   </si>
   <si>
-    <t>PathFileResult</t>
-  </si>
-  <si>
     <t>C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Data\Temp\Price List to date.xlsx</t>
   </si>
   <si>
@@ -393,9 +390,6 @@
     <t>C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Data\Temp\Inventario to date.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Data\Temp\Status_Report AMA 2021.xlsx&gt;BASE</t>
-  </si>
-  <si>
     <t>C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Data\Temp\1.Generador Open Orders (Macro).xls</t>
   </si>
   <si>
@@ -409,17 +403,39 @@
   </si>
   <si>
     <t>7:30 - 9:29</t>
+  </si>
+  <si>
+    <t>ExtraData</t>
+  </si>
+  <si>
+    <t>C:\Users\rpalatam\Documents\UiPath\Proceso de Descarga de Reportes Diarios Customer Service\Data\Temp\Status_Report AMA 2021.xlsx</t>
+  </si>
+  <si>
+    <t>BASE;76;{28,29,30,40,41,45,67,68,69,70};A:BX</t>
+  </si>
+  <si>
+    <t>Base de datos;30;{19};A:AD</t>
+  </si>
+  <si>
+    <t>Base de datos;32;{7,9};A:AF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -595,16 +611,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -625,23 +641,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -650,23 +660,26 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,8 +688,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -684,14 +700,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2135,7 +2151,7 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="16"/>
+  <phoneticPr fontId="17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3299,7 +3315,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="16"/>
+  <phoneticPr fontId="17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4390,7 +4406,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="16"/>
+  <phoneticPr fontId="17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4498,7 +4514,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4509,7 +4525,7 @@
     <col min="5" max="5" width="16.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23" style="27" customWidth="1"/>
+    <col min="8" max="8" width="23" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4523,7 +4539,7 @@
         <v>75</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>93</v>
@@ -4531,71 +4547,73 @@
       <c r="F1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="60">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="18">
-        <v>1</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="28"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="60">
       <c r="A3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="16"/>
+      <c r="C3" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="E3" s="15">
         <v>2</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="H3" s="28"/>
+      <c r="G3" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="27"/>
     </row>
-    <row r="4" spans="1:8" ht="60">
+    <row r="4" spans="1:8" ht="45">
       <c r="A4" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>113</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="E4" s="15">
         <v>3</v>
@@ -4603,10 +4621,10 @@
       <c r="F4" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="H4" s="29" t="s">
+      <c r="G4" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="28" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4617,11 +4635,11 @@
       <c r="B5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>115</v>
+      <c r="D5" s="29" t="s">
+        <v>114</v>
       </c>
       <c r="E5" s="15">
         <v>3</v>
@@ -4629,10 +4647,10 @@
       <c r="F5" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4643,11 +4661,11 @@
       <c r="B6" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>116</v>
+      <c r="D6" s="29" t="s">
+        <v>115</v>
       </c>
       <c r="E6" s="15">
         <v>3</v>
@@ -4655,10 +4673,10 @@
       <c r="F6" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4669,37 +4687,37 @@
       <c r="B7" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>117</v>
+      <c r="D7" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="E7" s="13">
         <v>3</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="H7" s="28" t="s">
+      <c r="G7" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="27" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:8" ht="45">
+      <c r="A8" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>118</v>
+      <c r="C8" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>126</v>
       </c>
       <c r="E8" s="15">
         <v>3</v>
@@ -4707,10 +4725,10 @@
       <c r="F8" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="27" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>